<commit_message>
data indexing (pre con, perf, con-perf)
</commit_message>
<xml_diff>
--- a/conversation/Present-Perfect-Continuous.xlsx
+++ b/conversation/Present-Perfect-Continuous.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\เบ็ดเตล็ด\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Pictures\Jiw\Project\grammar-police-game\testgame\conversation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DC2614-D94F-4600-B619-33F3DF21B0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA91703-2330-4D2E-B165-E32D1CFD7C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A118E7C0-E6DA-445D-BF73-F525DA469D57}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A118E7C0-E6DA-445D-BF73-F525DA469D57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="79">
   <si>
     <t>ID</t>
   </si>
@@ -107,15 +105,9 @@
     <t>No, she's still deciding on the best dates for her trip.</t>
   </si>
   <si>
-    <t>are</t>
-  </si>
-  <si>
     <t>is</t>
   </si>
   <si>
-    <t>studied</t>
-  </si>
-  <si>
     <t>studying</t>
   </si>
   <si>
@@ -126,7 +118,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -136,7 +128,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -152,7 +144,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -162,7 +154,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -171,9 +163,6 @@
     </r>
   </si>
   <si>
-    <t>Have</t>
-  </si>
-  <si>
     <t>Has</t>
   </si>
   <si>
@@ -184,7 +173,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -194,7 +183,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -209,9 +198,6 @@
     <t>doing</t>
   </si>
   <si>
-    <t>do</t>
-  </si>
-  <si>
     <r>
       <t>What have you been</t>
     </r>
@@ -219,7 +205,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -229,7 +215,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -238,9 +224,6 @@
     </r>
   </si>
   <si>
-    <t>worked</t>
-  </si>
-  <si>
     <t>working</t>
   </si>
   <si>
@@ -251,7 +234,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -261,7 +244,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -283,7 +266,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -293,7 +276,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -302,9 +285,6 @@
     </r>
   </si>
   <si>
-    <t>felt</t>
-  </si>
-  <si>
     <t>feeling</t>
   </si>
   <si>
@@ -315,7 +295,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -325,7 +305,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -334,9 +314,6 @@
     </r>
   </si>
   <si>
-    <t>seen</t>
-  </si>
-  <si>
     <t>seeing</t>
   </si>
   <si>
@@ -347,7 +324,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -357,7 +334,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -376,7 +353,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -386,7 +363,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -395,15 +372,9 @@
     </r>
   </si>
   <si>
-    <t>play</t>
-  </si>
-  <si>
     <t>playing</t>
   </si>
   <si>
-    <t>practiced</t>
-  </si>
-  <si>
     <t>praticing</t>
   </si>
   <si>
@@ -414,7 +385,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -424,7 +395,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -440,7 +411,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -450,7 +421,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -463,7 +434,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -473,7 +444,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -482,9 +453,6 @@
     </r>
   </si>
   <si>
-    <t>thought</t>
-  </si>
-  <si>
     <t>thinking</t>
   </si>
   <si>
@@ -495,7 +463,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -505,7 +473,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -514,9 +482,6 @@
     </r>
   </si>
   <si>
-    <t>try</t>
-  </si>
-  <si>
     <t>trying</t>
   </si>
   <si>
@@ -527,7 +492,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -537,7 +502,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -556,7 +521,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -566,7 +531,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -575,12 +540,6 @@
     </r>
   </si>
   <si>
-    <t>meant</t>
-  </si>
-  <si>
-    <t>go</t>
-  </si>
-  <si>
     <t>going</t>
   </si>
   <si>
@@ -591,7 +550,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -601,7 +560,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -610,9 +569,6 @@
     </r>
   </si>
   <si>
-    <t>heard</t>
-  </si>
-  <si>
     <t>hearing</t>
   </si>
   <si>
@@ -623,7 +579,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -633,7 +589,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -642,9 +598,6 @@
     </r>
   </si>
   <si>
-    <t>gone</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">It's been </t>
     </r>
@@ -652,7 +605,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -662,7 +615,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -678,7 +631,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -688,7 +641,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -697,9 +650,6 @@
     </r>
   </si>
   <si>
-    <t>look</t>
-  </si>
-  <si>
     <t>looking</t>
   </si>
   <si>
@@ -710,7 +660,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -720,7 +670,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -729,9 +679,6 @@
     </r>
   </si>
   <si>
-    <t>planned</t>
-  </si>
-  <si>
     <t>planning</t>
   </si>
   <si>
@@ -742,7 +689,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -752,7 +699,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -768,7 +715,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -778,7 +725,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -787,9 +734,6 @@
     </r>
   </si>
   <si>
-    <t>driven</t>
-  </si>
-  <si>
     <t>driving</t>
   </si>
   <si>
@@ -800,7 +744,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -810,7 +754,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -819,9 +763,6 @@
     </r>
   </si>
   <si>
-    <t>studies</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">How long have you been </t>
     </r>
@@ -829,7 +770,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -839,7 +780,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -855,7 +796,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -865,7 +806,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -874,9 +815,6 @@
     </r>
   </si>
   <si>
-    <t>prepared</t>
-  </si>
-  <si>
     <t>preparing</t>
   </si>
   <si>
@@ -887,7 +825,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -897,7 +835,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -906,9 +844,6 @@
     </r>
   </si>
   <si>
-    <t>eaten</t>
-  </si>
-  <si>
     <t>eating</t>
   </si>
   <si>
@@ -919,7 +854,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -929,7 +864,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -945,7 +880,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -955,7 +890,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -964,9 +899,6 @@
     </r>
   </si>
   <si>
-    <t>explored</t>
-  </si>
-  <si>
     <t>exploring</t>
   </si>
   <si>
@@ -977,7 +909,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -987,7 +919,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -1006,7 +938,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1016,7 +948,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -1025,9 +957,6 @@
     </r>
   </si>
   <si>
-    <t>played</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">I've been </t>
     </r>
@@ -1035,7 +964,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1045,7 +974,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="222"/>
         <scheme val="minor"/>
@@ -1062,7 +991,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -1070,14 +999,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Tahoma"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1115,7 +1044,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1449,18 +1378,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7E8811B-44DC-42BF-A74A-70165A61B52B}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="128" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="128" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="2" width="8.6640625" style="1"/>
     <col min="3" max="3" width="25.33203125" style="2" customWidth="1"/>
     <col min="4" max="5" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1477,7 +1406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1486,16 +1415,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="56" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" ht="66" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <f t="shared" ref="A3:A4" si="0">A2</f>
         <v>1</v>
@@ -1505,16 +1434,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1524,16 +1453,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="D4" s="1">
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1543,14 +1472,14 @@
       <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>32</v>
+      <c r="D5" s="1">
+        <v>-1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -1559,16 +1488,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="84" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="82.5" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <f t="shared" ref="A7:A8" si="3">A6</f>
         <v>2</v>
@@ -1578,16 +1507,16 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -1599,14 +1528,14 @@
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>32</v>
+      <c r="D8" s="1">
+        <v>-1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -1614,16 +1543,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -1632,16 +1561,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="70" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="82.5" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <f t="shared" ref="A11:A12" si="5">A10</f>
         <v>3</v>
@@ -1651,16 +1580,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="D11" s="1">
+        <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <f t="shared" si="5"/>
         <v>3</v>
@@ -1672,14 +1601,14 @@
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>32</v>
+      <c r="D12" s="1">
+        <v>-1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -1687,16 +1616,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>4</v>
       </c>
@@ -1705,16 +1634,16 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="70" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="82.5" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <f t="shared" ref="A15:A16" si="7">A14</f>
         <v>4</v>
@@ -1726,14 +1655,14 @@
       <c r="C15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>32</v>
+      <c r="D15" s="1">
+        <v>-1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <f t="shared" si="7"/>
         <v>4</v>
@@ -1743,16 +1672,16 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>4</v>
       </c>
@@ -1760,16 +1689,16 @@
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>5</v>
       </c>
@@ -1778,16 +1707,16 @@
         <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="70" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="82.5" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <f t="shared" ref="A19:A20" si="9">A18</f>
         <v>5</v>
@@ -1797,16 +1726,16 @@
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
+      </c>
+      <c r="D19" s="1">
+        <v>13</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <f t="shared" si="9"/>
         <v>5</v>
@@ -1818,14 +1747,14 @@
       <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>32</v>
+      <c r="D20" s="1">
+        <v>-1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>5</v>
       </c>
@@ -1835,14 +1764,14 @@
       <c r="C21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>32</v>
+      <c r="D21" s="1">
+        <v>-1</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>6</v>
       </c>
@@ -1853,14 +1782,14 @@
       <c r="C22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>32</v>
+      <c r="D22" s="1">
+        <v>-1</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <f t="shared" ref="A23:A24" si="11">A22</f>
         <v>6</v>
@@ -1872,14 +1801,14 @@
       <c r="C23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>32</v>
+      <c r="D23" s="1">
+        <v>-1</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <f t="shared" si="11"/>
         <v>6</v>
@@ -1889,16 +1818,16 @@
         <v>3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
+      </c>
+      <c r="D24" s="1">
+        <v>5</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>7</v>
       </c>
@@ -1909,14 +1838,14 @@
       <c r="C25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>32</v>
+      <c r="D25" s="1">
+        <v>-1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <f t="shared" ref="A26:A27" si="13">A25</f>
         <v>7</v>
@@ -1926,16 +1855,16 @@
         <v>2</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
+      </c>
+      <c r="D26" s="1">
+        <v>5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <f t="shared" si="13"/>
         <v>7</v>
@@ -1945,16 +1874,16 @@
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
+      </c>
+      <c r="D27" s="1">
+        <v>4</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>8</v>
       </c>
@@ -1965,14 +1894,14 @@
       <c r="C28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>32</v>
+      <c r="D28" s="1">
+        <v>-1</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <f t="shared" ref="A29:A30" si="15">A28</f>
         <v>8</v>
@@ -1982,16 +1911,16 @@
         <v>2</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
+      </c>
+      <c r="D29" s="1">
+        <v>8</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="56" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="66" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <f t="shared" si="15"/>
         <v>8</v>
@@ -2003,14 +1932,14 @@
       <c r="C30" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>32</v>
+      <c r="D30" s="1">
+        <v>-1</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>9</v>
       </c>
@@ -2021,14 +1950,14 @@
       <c r="C31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>32</v>
+      <c r="D31" s="1">
+        <v>-1</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="56" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="66" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <f t="shared" ref="A32:A33" si="17">A31</f>
         <v>9</v>
@@ -2038,16 +1967,16 @@
         <v>2</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <f t="shared" si="17"/>
         <v>9</v>
@@ -2057,16 +1986,16 @@
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>10</v>
       </c>
@@ -2077,14 +2006,14 @@
       <c r="C34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>32</v>
+      <c r="D34" s="1">
+        <v>-1</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <f t="shared" ref="A35:A36" si="19">A34</f>
         <v>10</v>
@@ -2094,16 +2023,16 @@
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>75</v>
+        <v>61</v>
+      </c>
+      <c r="D35" s="1">
+        <v>5</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <f t="shared" si="19"/>
         <v>10</v>
@@ -2113,16 +2042,16 @@
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>78</v>
+        <v>63</v>
+      </c>
+      <c r="D36" s="1">
+        <v>8</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>11</v>
       </c>
@@ -2131,16 +2060,16 @@
         <v>1</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <f t="shared" ref="A38:A39" si="21">A37</f>
         <v>11</v>
@@ -2150,16 +2079,16 @@
         <v>2</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>82</v>
+        <v>66</v>
+      </c>
+      <c r="D38" s="1">
+        <v>9</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <f t="shared" si="21"/>
         <v>11</v>
@@ -2171,14 +2100,14 @@
       <c r="C39" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>32</v>
+      <c r="D39" s="1">
+        <v>-1</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>12</v>
       </c>
@@ -2187,16 +2116,16 @@
         <v>1</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
+      </c>
+      <c r="D40" s="1">
+        <v>5</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <f t="shared" ref="A41:A42" si="23">A40</f>
         <v>12</v>
@@ -2206,16 +2135,16 @@
         <v>2</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>39</v>
+        <v>68</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <f t="shared" si="23"/>
         <v>12</v>
@@ -2225,16 +2154,16 @@
         <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>88</v>
+        <v>70</v>
+      </c>
+      <c r="D42" s="1">
+        <v>7</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>13</v>
       </c>
@@ -2243,16 +2172,16 @@
         <v>1</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>91</v>
+        <v>72</v>
+      </c>
+      <c r="D43" s="1">
+        <v>4</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <f t="shared" ref="A44:A45" si="25">A43</f>
         <v>13</v>
@@ -2264,14 +2193,14 @@
       <c r="C44" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>32</v>
+      <c r="D44" s="1">
+        <v>-1</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <f t="shared" si="25"/>
         <v>13</v>
@@ -2283,14 +2212,14 @@
       <c r="C45" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>32</v>
+      <c r="D45" s="1">
+        <v>-1</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>14</v>
       </c>
@@ -2299,16 +2228,16 @@
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>39</v>
+        <v>73</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <f t="shared" ref="A47:A48" si="27">A46</f>
         <v>14</v>
@@ -2318,16 +2247,16 @@
         <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>95</v>
+        <v>75</v>
+      </c>
+      <c r="D47" s="1">
+        <v>2</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <f t="shared" si="27"/>
         <v>14</v>
@@ -2339,14 +2268,14 @@
       <c r="C48" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>32</v>
+      <c r="D48" s="1">
+        <v>-1</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>14</v>
       </c>
@@ -2354,16 +2283,16 @@
         <v>4</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>32</v>
+        <v>76</v>
+      </c>
+      <c r="D49" s="1">
+        <v>-1</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>15</v>
       </c>
@@ -2372,16 +2301,16 @@
         <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>34</v>
+        <v>77</v>
+      </c>
+      <c r="D50" s="1">
+        <v>2</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="49.5" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <f t="shared" ref="A51:A52" si="29">A50</f>
         <v>15</v>
@@ -2391,16 +2320,16 @@
         <v>2</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>100</v>
+        <v>78</v>
+      </c>
+      <c r="D51" s="1">
+        <v>2</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="56" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="66" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <f t="shared" si="29"/>
         <v>15</v>
@@ -2412,11 +2341,11 @@
       <c r="C52" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>32</v>
+      <c r="D52" s="1">
+        <v>-1</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>